<commit_message>
fixed issues and testing
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -435,13 +435,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -450,13 +450,13 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2135355.308333333</v>
+        <v>2510362.816666667</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -465,13 +465,13 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -480,13 +480,13 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -495,13 +495,13 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>2135355.308333333</v>
+        <v>2343005.295555555</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -510,13 +510,13 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -525,13 +525,13 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2135355.308333333</v>
+        <v>2510362.816666667</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -540,13 +540,13 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -555,13 +555,13 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>2206533.818611111</v>
+        <v>2510362.816666667</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -570,13 +570,13 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>1992998.287777778</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -585,13 +585,13 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -600,13 +600,13 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>2135355.308333333</v>
+        <v>2510362.816666667</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -615,13 +615,13 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -630,13 +630,13 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>2135355.308333333</v>
+        <v>2510362.816666667</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -645,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -660,13 +660,13 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -675,13 +675,13 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>2135355.308333333</v>
+        <v>2343005.295555555</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -690,13 +690,13 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -705,13 +705,13 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>2135355.308333333</v>
+        <v>2510362.816666667</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -720,13 +720,13 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -735,13 +735,13 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>2206533.818611111</v>
+        <v>2510362.816666667</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -750,13 +750,13 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>1992998.287777778</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -765,13 +765,13 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>2206533.818611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>342113000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -780,13 +780,13 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>2135355.308333333</v>
+        <v>2510362.816666667</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>321449000</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -795,13 +795,13 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>2073256.758611111</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>280307088.48</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -810,13 +810,13 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <v>1749583.410596</v>
+        <v>2510362.816666667</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>280307088.48</v>
+        <v>431581000</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -825,13 +825,13 @@
         <v>26</v>
       </c>
       <c r="C28">
-        <v>1807902.857615867</v>
+        <v>2594041.577222222</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>29520096.52</v>
       </c>
       <c r="E28">
-        <v>275533288.48</v>
+        <v>402060903.48</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -840,13 +840,13 @@
         <v>27</v>
       </c>
       <c r="C29">
-        <v>1777113.173671422</v>
+        <v>2416609.3970834</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>199166831.7</v>
+        <v>402060903.48</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -855,13 +855,13 @@
         <v>28</v>
       </c>
       <c r="C30">
-        <v>1243132.9745275</v>
+        <v>2182743.9715592</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>199166831.7</v>
+        <v>402060903.48</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -870,13 +870,13 @@
         <v>29</v>
       </c>
       <c r="C31">
-        <v>1284570.740345083</v>
+        <v>2416609.3970834</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>175653524.22</v>
+        <v>402060903.48</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -885,13 +885,13 @@
         <v>30</v>
       </c>
       <c r="C32">
-        <v>1096370.7470065</v>
+        <v>2338654.255242</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>24726890.72</v>
       </c>
       <c r="E32">
-        <v>175653524.22</v>
+        <v>377334012.76</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -900,13 +900,13 @@
         <v>31</v>
       </c>
       <c r="C33">
-        <v>1132916.438573383</v>
+        <v>2267987.046694688</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>93893852.33</v>
       </c>
       <c r="E33">
-        <v>149998434.83</v>
+        <v>283440160.4300001</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -915,13 +915,13 @@
         <v>32</v>
       </c>
       <c r="C34">
-        <v>967448.238421603</v>
+        <v>1648676.933167834</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>122437492.78</v>
+        <v>283440160.4300001</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -930,13 +930,13 @@
         <v>33</v>
       </c>
       <c r="C35">
-        <v>713266.4162728223</v>
+        <v>1703632.830940095</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>72080000</v>
       </c>
       <c r="E35">
-        <v>122437492.78</v>
+        <v>211360160.4300001</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -945,13 +945,13 @@
         <v>34</v>
       </c>
       <c r="C36">
-        <v>789687.818016339</v>
+        <v>1270391.98649565</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>65546472.98000004</v>
+        <v>211360160.4300001</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -960,13 +960,13 @@
         <v>35</v>
       </c>
       <c r="C37">
-        <v>409119.2355168335</v>
+        <v>1229411.5998345</v>
       </c>
       <c r="D37">
-        <v>65546472.98000004</v>
+        <v>53017000</v>
       </c>
       <c r="E37">
-        <v>24187463.16000004</v>
+        <v>158343160.4300001</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -975,13 +975,13 @@
         <v>36</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>951730.3626067615</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>158343160.4300001</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -990,13 +990,13 @@
         <v>37</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>921029.3831678338</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>158343160.4300001</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1005,13 +1005,13 @@
         <v>38</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>951730.3626067615</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>158343160.4300001</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1020,13 +1020,13 @@
         <v>39</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>951730.3626067615</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>13267459.11</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>145075701.3200001</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1035,13 +1035,13 @@
         <v>40</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>787599.8629439113</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>145075701.3200001</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1050,13 +1050,13 @@
         <v>41</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>871985.5625450449</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>145075701.3200001</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1065,13 +1065,13 @@
         <v>42</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>843856.9960113337</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>17235701.32000005</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1080,10 +1080,10 @@
         <v>43</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>103596.1403228225</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>17235701.32000005</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1337,13 +1337,13 @@
         <v>0</v>
       </c>
       <c r="C62">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="E62">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1352,13 +1352,13 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>693850.2083333333</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1367,13 +1367,13 @@
         <v>2</v>
       </c>
       <c r="C64">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
       <c r="E64">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1382,13 +1382,13 @@
         <v>3</v>
       </c>
       <c r="C65">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
       <c r="E65">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1397,13 +1397,13 @@
         <v>4</v>
       </c>
       <c r="C66">
-        <v>693850.2083333333</v>
+        <v>664544.4244444444</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1412,13 +1412,13 @@
         <v>5</v>
       </c>
       <c r="C67">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
       <c r="E67">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1427,13 +1427,13 @@
         <v>6</v>
       </c>
       <c r="C68">
-        <v>693850.2083333333</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D68">
         <v>0</v>
       </c>
       <c r="E68">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1442,13 +1442,13 @@
         <v>7</v>
       </c>
       <c r="C69">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D69">
         <v>0</v>
       </c>
       <c r="E69">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1457,13 +1457,13 @@
         <v>8</v>
       </c>
       <c r="C70">
-        <v>716978.548611111</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D70">
         <v>0</v>
       </c>
       <c r="E70">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1472,13 +1472,13 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>647593.5277777778</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1487,13 +1487,13 @@
         <v>10</v>
       </c>
       <c r="C72">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
       <c r="E72">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1502,13 +1502,13 @@
         <v>11</v>
       </c>
       <c r="C73">
-        <v>693850.2083333333</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1517,13 +1517,13 @@
         <v>12</v>
       </c>
       <c r="C74">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D74">
         <v>0</v>
       </c>
       <c r="E74">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1532,13 +1532,13 @@
         <v>13</v>
       </c>
       <c r="C75">
-        <v>693850.2083333333</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D75">
         <v>0</v>
       </c>
       <c r="E75">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1547,13 +1547,13 @@
         <v>14</v>
       </c>
       <c r="C76">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D76">
         <v>0</v>
       </c>
       <c r="E76">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1562,13 +1562,13 @@
         <v>15</v>
       </c>
       <c r="C77">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D77">
         <v>0</v>
       </c>
       <c r="E77">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1577,13 +1577,13 @@
         <v>16</v>
       </c>
       <c r="C78">
-        <v>693850.2083333333</v>
+        <v>664544.4244444444</v>
       </c>
       <c r="D78">
         <v>0</v>
       </c>
       <c r="E78">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1592,13 +1592,13 @@
         <v>17</v>
       </c>
       <c r="C79">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1607,13 +1607,13 @@
         <v>18</v>
       </c>
       <c r="C80">
-        <v>693850.2083333333</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D80">
         <v>0</v>
       </c>
       <c r="E80">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1622,13 +1622,13 @@
         <v>19</v>
       </c>
       <c r="C81">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D81">
         <v>0</v>
       </c>
       <c r="E81">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1637,13 +1637,13 @@
         <v>20</v>
       </c>
       <c r="C82">
-        <v>716978.548611111</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D82">
         <v>0</v>
       </c>
       <c r="E82">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1652,13 +1652,13 @@
         <v>21</v>
       </c>
       <c r="C83">
-        <v>647593.5277777778</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D83">
         <v>0</v>
       </c>
       <c r="E83">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1667,13 +1667,13 @@
         <v>22</v>
       </c>
       <c r="C84">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D84">
         <v>0</v>
       </c>
       <c r="E84">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1682,13 +1682,13 @@
         <v>23</v>
       </c>
       <c r="C85">
-        <v>693850.2083333333</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D85">
         <v>0</v>
       </c>
       <c r="E85">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1697,13 +1697,13 @@
         <v>24</v>
       </c>
       <c r="C86">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
       <c r="E86">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -1712,13 +1712,13 @@
         <v>25</v>
       </c>
       <c r="C87">
-        <v>693850.2083333333</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D87">
         <v>0</v>
       </c>
       <c r="E87">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1727,13 +1727,13 @@
         <v>26</v>
       </c>
       <c r="C88">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
       <c r="E88">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1742,13 +1742,13 @@
         <v>27</v>
       </c>
       <c r="C89">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D89">
         <v>0</v>
       </c>
       <c r="E89">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1757,13 +1757,13 @@
         <v>28</v>
       </c>
       <c r="C90">
-        <v>693850.2083333333</v>
+        <v>664544.4244444444</v>
       </c>
       <c r="D90">
         <v>0</v>
       </c>
       <c r="E90">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -1772,13 +1772,13 @@
         <v>29</v>
       </c>
       <c r="C91">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
       <c r="E91">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -1787,13 +1787,13 @@
         <v>30</v>
       </c>
       <c r="C92">
-        <v>693850.2083333333</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D92">
         <v>0</v>
       </c>
       <c r="E92">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -1802,13 +1802,13 @@
         <v>31</v>
       </c>
       <c r="C93">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D93">
         <v>0</v>
       </c>
       <c r="E93">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -1817,13 +1817,13 @@
         <v>32</v>
       </c>
       <c r="C94">
-        <v>716978.548611111</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D94">
         <v>0</v>
       </c>
       <c r="E94">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -1832,13 +1832,13 @@
         <v>33</v>
       </c>
       <c r="C95">
-        <v>647593.5277777778</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D95">
         <v>0</v>
       </c>
       <c r="E95">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -1847,13 +1847,13 @@
         <v>34</v>
       </c>
       <c r="C96">
-        <v>716978.548611111</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D96">
         <v>0</v>
       </c>
       <c r="E96">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -1862,13 +1862,13 @@
         <v>35</v>
       </c>
       <c r="C97">
-        <v>693850.2083333333</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D97">
-        <v>99715000</v>
+        <v>0</v>
       </c>
       <c r="E97">
-        <v>99715000</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -1877,13 +1877,13 @@
         <v>36</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D98">
         <v>0</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -1892,13 +1892,13 @@
         <v>37</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D99">
         <v>0</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -1907,13 +1907,13 @@
         <v>38</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D100">
         <v>0</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -1922,13 +1922,13 @@
         <v>39</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D101">
         <v>0</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -1937,13 +1937,13 @@
         <v>40</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>664544.4244444444</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -1952,13 +1952,13 @@
         <v>41</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D103">
         <v>0</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -1967,13 +1967,13 @@
         <v>42</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>712011.8833333333</v>
       </c>
       <c r="D104">
         <v>0</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>114074000</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -1982,13 +1982,13 @@
         <v>43</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>735745.6127777777</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>114074000</v>
       </c>
       <c r="E105">
-        <v>0</v>
+        <v>58569843.69000006</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2239,13 +2239,13 @@
         <v>0</v>
       </c>
       <c r="C122">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D122">
         <v>0</v>
       </c>
       <c r="E122">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2254,13 +2254,13 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>221220.5</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D123">
         <v>0</v>
       </c>
       <c r="E123">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -2269,13 +2269,13 @@
         <v>2</v>
       </c>
       <c r="C124">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D124">
         <v>0</v>
       </c>
       <c r="E124">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -2284,13 +2284,13 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D125">
         <v>0</v>
       </c>
       <c r="E125">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -2299,13 +2299,13 @@
         <v>4</v>
       </c>
       <c r="C126">
-        <v>221220.5</v>
+        <v>284826.6322222222</v>
       </c>
       <c r="D126">
         <v>0</v>
       </c>
       <c r="E126">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -2314,13 +2314,13 @@
         <v>5</v>
       </c>
       <c r="C127">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D127">
         <v>0</v>
       </c>
       <c r="E127">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -2329,13 +2329,13 @@
         <v>6</v>
       </c>
       <c r="C128">
-        <v>221220.5</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D128">
         <v>0</v>
       </c>
       <c r="E128">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -2344,13 +2344,13 @@
         <v>7</v>
       </c>
       <c r="C129">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D129">
         <v>0</v>
       </c>
       <c r="E129">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -2359,13 +2359,13 @@
         <v>8</v>
       </c>
       <c r="C130">
-        <v>228594.5166666667</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D130">
         <v>0</v>
       </c>
       <c r="E130">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -2374,13 +2374,13 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>206472.4666666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D131">
         <v>0</v>
       </c>
       <c r="E131">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -2389,13 +2389,13 @@
         <v>10</v>
       </c>
       <c r="C132">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D132">
         <v>0</v>
       </c>
       <c r="E132">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -2404,13 +2404,13 @@
         <v>11</v>
       </c>
       <c r="C133">
-        <v>221220.5</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D133">
         <v>0</v>
       </c>
       <c r="E133">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -2419,13 +2419,13 @@
         <v>12</v>
       </c>
       <c r="C134">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D134">
         <v>0</v>
       </c>
       <c r="E134">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -2434,13 +2434,13 @@
         <v>13</v>
       </c>
       <c r="C135">
-        <v>221220.5</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D135">
         <v>0</v>
       </c>
       <c r="E135">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -2449,13 +2449,13 @@
         <v>14</v>
       </c>
       <c r="C136">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D136">
         <v>0</v>
       </c>
       <c r="E136">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -2464,13 +2464,13 @@
         <v>15</v>
       </c>
       <c r="C137">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D137">
         <v>0</v>
       </c>
       <c r="E137">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -2479,13 +2479,13 @@
         <v>16</v>
       </c>
       <c r="C138">
-        <v>221220.5</v>
+        <v>284826.6322222222</v>
       </c>
       <c r="D138">
         <v>0</v>
       </c>
       <c r="E138">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -2494,13 +2494,13 @@
         <v>17</v>
       </c>
       <c r="C139">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D139">
         <v>0</v>
       </c>
       <c r="E139">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -2509,13 +2509,13 @@
         <v>18</v>
       </c>
       <c r="C140">
-        <v>221220.5</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D140">
         <v>0</v>
       </c>
       <c r="E140">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -2524,13 +2524,13 @@
         <v>19</v>
       </c>
       <c r="C141">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D141">
         <v>0</v>
       </c>
       <c r="E141">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -2539,13 +2539,13 @@
         <v>20</v>
       </c>
       <c r="C142">
-        <v>228594.5166666667</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D142">
         <v>0</v>
       </c>
       <c r="E142">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -2554,13 +2554,13 @@
         <v>21</v>
       </c>
       <c r="C143">
-        <v>206472.4666666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D143">
         <v>0</v>
       </c>
       <c r="E143">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -2569,13 +2569,13 @@
         <v>22</v>
       </c>
       <c r="C144">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D144">
         <v>0</v>
       </c>
       <c r="E144">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -2584,13 +2584,13 @@
         <v>23</v>
       </c>
       <c r="C145">
-        <v>221220.5</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D145">
         <v>0</v>
       </c>
       <c r="E145">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -2599,13 +2599,13 @@
         <v>24</v>
       </c>
       <c r="C146">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D146">
         <v>0</v>
       </c>
       <c r="E146">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -2614,13 +2614,13 @@
         <v>25</v>
       </c>
       <c r="C147">
-        <v>221220.5</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D147">
         <v>0</v>
       </c>
       <c r="E147">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -2629,13 +2629,13 @@
         <v>26</v>
       </c>
       <c r="C148">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D148">
         <v>0</v>
       </c>
       <c r="E148">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -2644,13 +2644,13 @@
         <v>27</v>
       </c>
       <c r="C149">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D149">
         <v>0</v>
       </c>
       <c r="E149">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -2659,13 +2659,13 @@
         <v>28</v>
       </c>
       <c r="C150">
-        <v>221220.5</v>
+        <v>284826.6322222222</v>
       </c>
       <c r="D150">
         <v>0</v>
       </c>
       <c r="E150">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -2674,13 +2674,13 @@
         <v>29</v>
       </c>
       <c r="C151">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D151">
         <v>0</v>
       </c>
       <c r="E151">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -2689,13 +2689,13 @@
         <v>30</v>
       </c>
       <c r="C152">
-        <v>221220.5</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D152">
         <v>0</v>
       </c>
       <c r="E152">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -2704,13 +2704,13 @@
         <v>31</v>
       </c>
       <c r="C153">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D153">
         <v>0</v>
       </c>
       <c r="E153">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -2719,13 +2719,13 @@
         <v>32</v>
       </c>
       <c r="C154">
-        <v>228594.5166666667</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D154">
         <v>0</v>
       </c>
       <c r="E154">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -2734,13 +2734,13 @@
         <v>33</v>
       </c>
       <c r="C155">
-        <v>206472.4666666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D155">
         <v>0</v>
       </c>
       <c r="E155">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -2749,13 +2749,13 @@
         <v>34</v>
       </c>
       <c r="C156">
-        <v>228594.5166666667</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D156">
         <v>0</v>
       </c>
       <c r="E156">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -2764,13 +2764,13 @@
         <v>35</v>
       </c>
       <c r="C157">
-        <v>221220.5</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D157">
-        <v>29996000</v>
+        <v>0</v>
       </c>
       <c r="E157">
-        <v>29996000</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -2779,13 +2779,13 @@
         <v>36</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D158">
         <v>0</v>
       </c>
       <c r="E158">
-        <v>0</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -2794,13 +2794,13 @@
         <v>37</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D159">
         <v>0</v>
       </c>
       <c r="E159">
-        <v>0</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -2809,13 +2809,13 @@
         <v>38</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D160">
         <v>0</v>
       </c>
       <c r="E160">
-        <v>0</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -2824,13 +2824,13 @@
         <v>39</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D161">
         <v>0</v>
       </c>
       <c r="E161">
-        <v>0</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -2839,13 +2839,13 @@
         <v>40</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>284826.6322222222</v>
       </c>
       <c r="D162">
         <v>0</v>
       </c>
       <c r="E162">
-        <v>0</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -2854,13 +2854,13 @@
         <v>41</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D163">
         <v>0</v>
       </c>
       <c r="E163">
-        <v>0</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -2869,13 +2869,13 @@
         <v>42</v>
       </c>
       <c r="C164">
-        <v>0</v>
+        <v>305171.3916666666</v>
       </c>
       <c r="D164">
         <v>0</v>
       </c>
       <c r="E164">
-        <v>0</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -2884,13 +2884,13 @@
         <v>43</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>315343.7713888889</v>
       </c>
       <c r="D165">
-        <v>0</v>
+        <v>45833000</v>
       </c>
       <c r="E165">
-        <v>0</v>
+        <v>45833000</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -3141,13 +3141,13 @@
         <v>0</v>
       </c>
       <c r="C182">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D182">
         <v>0</v>
       </c>
       <c r="E182">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -3156,13 +3156,13 @@
         <v>1</v>
       </c>
       <c r="C183">
-        <v>301443.6666666667</v>
+        <v>331914.55</v>
       </c>
       <c r="D183">
         <v>0</v>
       </c>
       <c r="E183">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -3171,13 +3171,13 @@
         <v>2</v>
       </c>
       <c r="C184">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D184">
         <v>0</v>
       </c>
       <c r="E184">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -3186,13 +3186,13 @@
         <v>3</v>
       </c>
       <c r="C185">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D185">
         <v>0</v>
       </c>
       <c r="E185">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -3201,13 +3201,13 @@
         <v>4</v>
       </c>
       <c r="C186">
-        <v>301443.6666666667</v>
+        <v>309786.9133333333</v>
       </c>
       <c r="D186">
         <v>0</v>
       </c>
       <c r="E186">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -3216,13 +3216,13 @@
         <v>5</v>
       </c>
       <c r="C187">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D187">
         <v>0</v>
       </c>
       <c r="E187">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -3231,13 +3231,13 @@
         <v>6</v>
       </c>
       <c r="C188">
-        <v>301443.6666666667</v>
+        <v>331914.55</v>
       </c>
       <c r="D188">
         <v>0</v>
       </c>
       <c r="E188">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -3246,13 +3246,13 @@
         <v>7</v>
       </c>
       <c r="C189">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D189">
         <v>0</v>
       </c>
       <c r="E189">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -3261,13 +3261,13 @@
         <v>8</v>
       </c>
       <c r="C190">
-        <v>311491.7888888889</v>
+        <v>331914.55</v>
       </c>
       <c r="D190">
         <v>0</v>
       </c>
       <c r="E190">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -3276,13 +3276,13 @@
         <v>9</v>
       </c>
       <c r="C191">
-        <v>281347.4222222222</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D191">
         <v>0</v>
       </c>
       <c r="E191">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -3291,13 +3291,13 @@
         <v>10</v>
       </c>
       <c r="C192">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D192">
         <v>0</v>
       </c>
       <c r="E192">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -3306,13 +3306,13 @@
         <v>11</v>
       </c>
       <c r="C193">
-        <v>301443.6666666667</v>
+        <v>331914.55</v>
       </c>
       <c r="D193">
         <v>0</v>
       </c>
       <c r="E193">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -3321,13 +3321,13 @@
         <v>12</v>
       </c>
       <c r="C194">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D194">
         <v>0</v>
       </c>
       <c r="E194">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -3336,13 +3336,13 @@
         <v>13</v>
       </c>
       <c r="C195">
-        <v>301443.6666666667</v>
+        <v>331914.55</v>
       </c>
       <c r="D195">
         <v>0</v>
       </c>
       <c r="E195">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -3351,13 +3351,13 @@
         <v>14</v>
       </c>
       <c r="C196">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D196">
         <v>0</v>
       </c>
       <c r="E196">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -3366,13 +3366,13 @@
         <v>15</v>
       </c>
       <c r="C197">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D197">
         <v>0</v>
       </c>
       <c r="E197">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -3381,13 +3381,13 @@
         <v>16</v>
       </c>
       <c r="C198">
-        <v>301443.6666666667</v>
+        <v>309786.9133333333</v>
       </c>
       <c r="D198">
         <v>0</v>
       </c>
       <c r="E198">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -3396,13 +3396,13 @@
         <v>17</v>
       </c>
       <c r="C199">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D199">
         <v>0</v>
       </c>
       <c r="E199">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -3411,13 +3411,13 @@
         <v>18</v>
       </c>
       <c r="C200">
-        <v>301443.6666666667</v>
+        <v>331914.55</v>
       </c>
       <c r="D200">
         <v>0</v>
       </c>
       <c r="E200">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -3426,13 +3426,13 @@
         <v>19</v>
       </c>
       <c r="C201">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D201">
         <v>0</v>
       </c>
       <c r="E201">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -3441,13 +3441,13 @@
         <v>20</v>
       </c>
       <c r="C202">
-        <v>311491.7888888889</v>
+        <v>331914.55</v>
       </c>
       <c r="D202">
         <v>0</v>
       </c>
       <c r="E202">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -3456,13 +3456,13 @@
         <v>21</v>
       </c>
       <c r="C203">
-        <v>281347.4222222222</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D203">
         <v>0</v>
       </c>
       <c r="E203">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -3471,13 +3471,13 @@
         <v>22</v>
       </c>
       <c r="C204">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D204">
         <v>0</v>
       </c>
       <c r="E204">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -3486,13 +3486,13 @@
         <v>23</v>
       </c>
       <c r="C205">
-        <v>301443.6666666667</v>
+        <v>331914.55</v>
       </c>
       <c r="D205">
         <v>0</v>
       </c>
       <c r="E205">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -3501,13 +3501,13 @@
         <v>24</v>
       </c>
       <c r="C206">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D206">
         <v>0</v>
       </c>
       <c r="E206">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -3516,13 +3516,13 @@
         <v>25</v>
       </c>
       <c r="C207">
-        <v>301443.6666666667</v>
+        <v>331914.55</v>
       </c>
       <c r="D207">
         <v>0</v>
       </c>
       <c r="E207">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -3531,13 +3531,13 @@
         <v>26</v>
       </c>
       <c r="C208">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D208">
         <v>0</v>
       </c>
       <c r="E208">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -3546,13 +3546,13 @@
         <v>27</v>
       </c>
       <c r="C209">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D209">
         <v>0</v>
       </c>
       <c r="E209">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -3561,13 +3561,13 @@
         <v>28</v>
       </c>
       <c r="C210">
-        <v>301443.6666666667</v>
+        <v>309786.9133333333</v>
       </c>
       <c r="D210">
         <v>0</v>
       </c>
       <c r="E210">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -3576,13 +3576,13 @@
         <v>29</v>
       </c>
       <c r="C211">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D211">
         <v>0</v>
       </c>
       <c r="E211">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -3591,13 +3591,13 @@
         <v>30</v>
       </c>
       <c r="C212">
-        <v>301443.6666666667</v>
+        <v>331914.55</v>
       </c>
       <c r="D212">
         <v>0</v>
       </c>
       <c r="E212">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -3606,13 +3606,13 @@
         <v>31</v>
       </c>
       <c r="C213">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D213">
         <v>0</v>
       </c>
       <c r="E213">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -3621,13 +3621,13 @@
         <v>32</v>
       </c>
       <c r="C214">
-        <v>311491.7888888889</v>
+        <v>331914.55</v>
       </c>
       <c r="D214">
         <v>0</v>
       </c>
       <c r="E214">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -3636,13 +3636,13 @@
         <v>33</v>
       </c>
       <c r="C215">
-        <v>281347.4222222222</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D215">
         <v>0</v>
       </c>
       <c r="E215">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -3651,13 +3651,13 @@
         <v>34</v>
       </c>
       <c r="C216">
-        <v>311491.7888888889</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D216">
         <v>0</v>
       </c>
       <c r="E216">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -3666,13 +3666,13 @@
         <v>35</v>
       </c>
       <c r="C217">
-        <v>301443.6666666667</v>
+        <v>331914.55</v>
       </c>
       <c r="D217">
-        <v>37292000</v>
+        <v>0</v>
       </c>
       <c r="E217">
-        <v>37292000</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -3681,13 +3681,13 @@
         <v>36</v>
       </c>
       <c r="C218">
-        <v>0</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D218">
         <v>0</v>
       </c>
       <c r="E218">
-        <v>0</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -3696,13 +3696,13 @@
         <v>37</v>
       </c>
       <c r="C219">
-        <v>0</v>
+        <v>331914.55</v>
       </c>
       <c r="D219">
         <v>0</v>
       </c>
       <c r="E219">
-        <v>0</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -3711,13 +3711,13 @@
         <v>38</v>
       </c>
       <c r="C220">
-        <v>0</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D220">
         <v>0</v>
       </c>
       <c r="E220">
-        <v>0</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -3726,13 +3726,13 @@
         <v>39</v>
       </c>
       <c r="C221">
-        <v>0</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D221">
         <v>0</v>
       </c>
       <c r="E221">
-        <v>0</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -3741,13 +3741,13 @@
         <v>40</v>
       </c>
       <c r="C222">
-        <v>0</v>
+        <v>309786.9133333333</v>
       </c>
       <c r="D222">
         <v>0</v>
       </c>
       <c r="E222">
-        <v>0</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -3756,13 +3756,13 @@
         <v>41</v>
       </c>
       <c r="C223">
-        <v>0</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D223">
         <v>0</v>
       </c>
       <c r="E223">
-        <v>0</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -3771,13 +3771,13 @@
         <v>42</v>
       </c>
       <c r="C224">
-        <v>0</v>
+        <v>331914.55</v>
       </c>
       <c r="D224">
         <v>0</v>
       </c>
       <c r="E224">
-        <v>0</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -3786,13 +3786,13 @@
         <v>43</v>
       </c>
       <c r="C225">
-        <v>0</v>
+        <v>342978.3683333333</v>
       </c>
       <c r="D225">
-        <v>0</v>
+        <v>45834000</v>
       </c>
       <c r="E225">
-        <v>0</v>
+        <v>45834000</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -4043,13 +4043,13 @@
         <v>0</v>
       </c>
       <c r="C242">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D242">
         <v>0</v>
       </c>
       <c r="E242">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="243" spans="1:5">
@@ -4058,13 +4058,13 @@
         <v>1</v>
       </c>
       <c r="C243">
-        <v>340488.75</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D243">
         <v>0</v>
       </c>
       <c r="E243">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="244" spans="1:5">
@@ -4073,13 +4073,13 @@
         <v>2</v>
       </c>
       <c r="C244">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D244">
         <v>0</v>
       </c>
       <c r="E244">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="245" spans="1:5">
@@ -4088,13 +4088,13 @@
         <v>3</v>
       </c>
       <c r="C245">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D245">
         <v>0</v>
       </c>
       <c r="E245">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="246" spans="1:5">
@@ -4103,13 +4103,13 @@
         <v>4</v>
       </c>
       <c r="C246">
-        <v>340488.75</v>
+        <v>279329.5944444445</v>
       </c>
       <c r="D246">
         <v>0</v>
       </c>
       <c r="E246">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="247" spans="1:5">
@@ -4118,13 +4118,13 @@
         <v>5</v>
       </c>
       <c r="C247">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D247">
         <v>0</v>
       </c>
       <c r="E247">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="248" spans="1:5">
@@ -4133,13 +4133,13 @@
         <v>6</v>
       </c>
       <c r="C248">
-        <v>340488.75</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D248">
         <v>0</v>
       </c>
       <c r="E248">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="249" spans="1:5">
@@ -4148,13 +4148,13 @@
         <v>7</v>
       </c>
       <c r="C249">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D249">
         <v>0</v>
       </c>
       <c r="E249">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="250" spans="1:5">
@@ -4163,13 +4163,13 @@
         <v>8</v>
       </c>
       <c r="C250">
-        <v>351838.375</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D250">
         <v>0</v>
       </c>
       <c r="E250">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="251" spans="1:5">
@@ -4178,13 +4178,13 @@
         <v>9</v>
       </c>
       <c r="C251">
-        <v>317789.5</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D251">
         <v>0</v>
       </c>
       <c r="E251">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="252" spans="1:5">
@@ -4193,13 +4193,13 @@
         <v>10</v>
       </c>
       <c r="C252">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D252">
         <v>0</v>
       </c>
       <c r="E252">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="253" spans="1:5">
@@ -4208,13 +4208,13 @@
         <v>11</v>
       </c>
       <c r="C253">
-        <v>340488.75</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D253">
         <v>0</v>
       </c>
       <c r="E253">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="254" spans="1:5">
@@ -4223,13 +4223,13 @@
         <v>12</v>
       </c>
       <c r="C254">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D254">
         <v>0</v>
       </c>
       <c r="E254">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="255" spans="1:5">
@@ -4238,13 +4238,13 @@
         <v>13</v>
       </c>
       <c r="C255">
-        <v>340488.75</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D255">
         <v>0</v>
       </c>
       <c r="E255">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="256" spans="1:5">
@@ -4253,13 +4253,13 @@
         <v>14</v>
       </c>
       <c r="C256">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D256">
         <v>0</v>
       </c>
       <c r="E256">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="257" spans="1:5">
@@ -4268,13 +4268,13 @@
         <v>15</v>
       </c>
       <c r="C257">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D257">
         <v>0</v>
       </c>
       <c r="E257">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="258" spans="1:5">
@@ -4283,13 +4283,13 @@
         <v>16</v>
       </c>
       <c r="C258">
-        <v>340488.75</v>
+        <v>279329.5944444445</v>
       </c>
       <c r="D258">
         <v>0</v>
       </c>
       <c r="E258">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="259" spans="1:5">
@@ -4298,13 +4298,13 @@
         <v>17</v>
       </c>
       <c r="C259">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D259">
         <v>0</v>
       </c>
       <c r="E259">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="260" spans="1:5">
@@ -4313,13 +4313,13 @@
         <v>18</v>
       </c>
       <c r="C260">
-        <v>340488.75</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D260">
         <v>0</v>
       </c>
       <c r="E260">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="261" spans="1:5">
@@ -4328,13 +4328,13 @@
         <v>19</v>
       </c>
       <c r="C261">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D261">
         <v>0</v>
       </c>
       <c r="E261">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="262" spans="1:5">
@@ -4343,13 +4343,13 @@
         <v>20</v>
       </c>
       <c r="C262">
-        <v>351838.375</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D262">
         <v>0</v>
       </c>
       <c r="E262">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="263" spans="1:5">
@@ -4358,13 +4358,13 @@
         <v>21</v>
       </c>
       <c r="C263">
-        <v>317789.5</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D263">
         <v>0</v>
       </c>
       <c r="E263">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="264" spans="1:5">
@@ -4373,13 +4373,13 @@
         <v>22</v>
       </c>
       <c r="C264">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D264">
         <v>0</v>
       </c>
       <c r="E264">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="265" spans="1:5">
@@ -4388,13 +4388,13 @@
         <v>23</v>
       </c>
       <c r="C265">
-        <v>340488.75</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D265">
         <v>0</v>
       </c>
       <c r="E265">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="266" spans="1:5">
@@ -4403,13 +4403,13 @@
         <v>24</v>
       </c>
       <c r="C266">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D266">
         <v>0</v>
       </c>
       <c r="E266">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="267" spans="1:5">
@@ -4418,13 +4418,13 @@
         <v>25</v>
       </c>
       <c r="C267">
-        <v>340488.75</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D267">
         <v>0</v>
       </c>
       <c r="E267">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="268" spans="1:5">
@@ -4433,13 +4433,13 @@
         <v>26</v>
       </c>
       <c r="C268">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D268">
         <v>0</v>
       </c>
       <c r="E268">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="269" spans="1:5">
@@ -4448,13 +4448,13 @@
         <v>27</v>
       </c>
       <c r="C269">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D269">
         <v>0</v>
       </c>
       <c r="E269">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="270" spans="1:5">
@@ -4463,13 +4463,13 @@
         <v>28</v>
       </c>
       <c r="C270">
-        <v>340488.75</v>
+        <v>279329.5944444445</v>
       </c>
       <c r="D270">
         <v>0</v>
       </c>
       <c r="E270">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="271" spans="1:5">
@@ -4478,13 +4478,13 @@
         <v>29</v>
       </c>
       <c r="C271">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D271">
         <v>0</v>
       </c>
       <c r="E271">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="272" spans="1:5">
@@ -4493,13 +4493,13 @@
         <v>30</v>
       </c>
       <c r="C272">
-        <v>340488.75</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D272">
         <v>0</v>
       </c>
       <c r="E272">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="273" spans="1:5">
@@ -4508,13 +4508,13 @@
         <v>31</v>
       </c>
       <c r="C273">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D273">
         <v>0</v>
       </c>
       <c r="E273">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="274" spans="1:5">
@@ -4523,13 +4523,13 @@
         <v>32</v>
       </c>
       <c r="C274">
-        <v>351838.375</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D274">
         <v>0</v>
       </c>
       <c r="E274">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="275" spans="1:5">
@@ -4538,13 +4538,13 @@
         <v>33</v>
       </c>
       <c r="C275">
-        <v>317789.5</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D275">
         <v>0</v>
       </c>
       <c r="E275">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="276" spans="1:5">
@@ -4553,13 +4553,13 @@
         <v>34</v>
       </c>
       <c r="C276">
-        <v>351838.375</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D276">
         <v>0</v>
       </c>
       <c r="E276">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="277" spans="1:5">
@@ -4568,13 +4568,13 @@
         <v>35</v>
       </c>
       <c r="C277">
-        <v>340488.75</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D277">
-        <v>38913000</v>
+        <v>0</v>
       </c>
       <c r="E277">
-        <v>38913000</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="278" spans="1:5">
@@ -4583,13 +4583,13 @@
         <v>36</v>
       </c>
       <c r="C278">
-        <v>0</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D278">
         <v>0</v>
       </c>
       <c r="E278">
-        <v>0</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="279" spans="1:5">
@@ -4598,13 +4598,13 @@
         <v>37</v>
       </c>
       <c r="C279">
-        <v>0</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D279">
         <v>0</v>
       </c>
       <c r="E279">
-        <v>0</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="280" spans="1:5">
@@ -4613,13 +4613,13 @@
         <v>38</v>
       </c>
       <c r="C280">
-        <v>0</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D280">
         <v>0</v>
       </c>
       <c r="E280">
-        <v>0</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="281" spans="1:5">
@@ -4628,13 +4628,13 @@
         <v>39</v>
       </c>
       <c r="C281">
-        <v>0</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D281">
         <v>0</v>
       </c>
       <c r="E281">
-        <v>0</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="282" spans="1:5">
@@ -4643,13 +4643,13 @@
         <v>40</v>
       </c>
       <c r="C282">
-        <v>0</v>
+        <v>279329.5944444445</v>
       </c>
       <c r="D282">
         <v>0</v>
       </c>
       <c r="E282">
-        <v>0</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="283" spans="1:5">
@@ -4658,13 +4658,13 @@
         <v>41</v>
       </c>
       <c r="C283">
-        <v>0</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D283">
         <v>0</v>
       </c>
       <c r="E283">
-        <v>0</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="284" spans="1:5">
@@ -4673,13 +4673,13 @@
         <v>42</v>
       </c>
       <c r="C284">
-        <v>0</v>
+        <v>299281.7083333333</v>
       </c>
       <c r="D284">
         <v>0</v>
       </c>
       <c r="E284">
-        <v>0</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="285" spans="1:5">
@@ -4688,13 +4688,13 @@
         <v>43</v>
       </c>
       <c r="C285">
-        <v>0</v>
+        <v>309257.7652777778</v>
       </c>
       <c r="D285">
-        <v>0</v>
+        <v>37685000</v>
       </c>
       <c r="E285">
-        <v>0</v>
+        <v>37685000</v>
       </c>
     </row>
     <row r="286" spans="1:5">
@@ -4945,13 +4945,13 @@
         <v>0</v>
       </c>
       <c r="C302">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D302">
         <v>0</v>
       </c>
       <c r="E302">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="303" spans="1:5">
@@ -4960,13 +4960,13 @@
         <v>1</v>
       </c>
       <c r="C303">
-        <v>100998.75</v>
+        <v>141639.4</v>
       </c>
       <c r="D303">
         <v>0</v>
       </c>
       <c r="E303">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="304" spans="1:5">
@@ -4975,13 +4975,13 @@
         <v>2</v>
       </c>
       <c r="C304">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D304">
         <v>0</v>
       </c>
       <c r="E304">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="305" spans="1:5">
@@ -4990,13 +4990,13 @@
         <v>3</v>
       </c>
       <c r="C305">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D305">
         <v>0</v>
       </c>
       <c r="E305">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="306" spans="1:5">
@@ -5005,13 +5005,13 @@
         <v>4</v>
       </c>
       <c r="C306">
-        <v>100998.75</v>
+        <v>132196.7733333333</v>
       </c>
       <c r="D306">
         <v>0</v>
       </c>
       <c r="E306">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="307" spans="1:5">
@@ -5020,13 +5020,13 @@
         <v>5</v>
       </c>
       <c r="C307">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D307">
         <v>0</v>
       </c>
       <c r="E307">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="308" spans="1:5">
@@ -5035,13 +5035,13 @@
         <v>6</v>
       </c>
       <c r="C308">
-        <v>100998.75</v>
+        <v>141639.4</v>
       </c>
       <c r="D308">
         <v>0</v>
       </c>
       <c r="E308">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="309" spans="1:5">
@@ -5050,13 +5050,13 @@
         <v>7</v>
       </c>
       <c r="C309">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D309">
         <v>0</v>
       </c>
       <c r="E309">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="310" spans="1:5">
@@ -5065,13 +5065,13 @@
         <v>8</v>
       </c>
       <c r="C310">
-        <v>104365.375</v>
+        <v>141639.4</v>
       </c>
       <c r="D310">
         <v>0</v>
       </c>
       <c r="E310">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="311" spans="1:5">
@@ -5080,13 +5080,13 @@
         <v>9</v>
       </c>
       <c r="C311">
-        <v>94265.5</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D311">
         <v>0</v>
       </c>
       <c r="E311">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="312" spans="1:5">
@@ -5095,13 +5095,13 @@
         <v>10</v>
       </c>
       <c r="C312">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D312">
         <v>0</v>
       </c>
       <c r="E312">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="313" spans="1:5">
@@ -5110,13 +5110,13 @@
         <v>11</v>
       </c>
       <c r="C313">
-        <v>100998.75</v>
+        <v>141639.4</v>
       </c>
       <c r="D313">
         <v>0</v>
       </c>
       <c r="E313">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="314" spans="1:5">
@@ -5125,13 +5125,13 @@
         <v>12</v>
       </c>
       <c r="C314">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D314">
         <v>0</v>
       </c>
       <c r="E314">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="315" spans="1:5">
@@ -5140,13 +5140,13 @@
         <v>13</v>
       </c>
       <c r="C315">
-        <v>100998.75</v>
+        <v>141639.4</v>
       </c>
       <c r="D315">
         <v>0</v>
       </c>
       <c r="E315">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="316" spans="1:5">
@@ -5155,13 +5155,13 @@
         <v>14</v>
       </c>
       <c r="C316">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D316">
         <v>0</v>
       </c>
       <c r="E316">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="317" spans="1:5">
@@ -5170,13 +5170,13 @@
         <v>15</v>
       </c>
       <c r="C317">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D317">
         <v>0</v>
       </c>
       <c r="E317">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="318" spans="1:5">
@@ -5185,13 +5185,13 @@
         <v>16</v>
       </c>
       <c r="C318">
-        <v>100998.75</v>
+        <v>132196.7733333333</v>
       </c>
       <c r="D318">
         <v>0</v>
       </c>
       <c r="E318">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="319" spans="1:5">
@@ -5200,13 +5200,13 @@
         <v>17</v>
       </c>
       <c r="C319">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D319">
         <v>0</v>
       </c>
       <c r="E319">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="320" spans="1:5">
@@ -5215,13 +5215,13 @@
         <v>18</v>
       </c>
       <c r="C320">
-        <v>100998.75</v>
+        <v>141639.4</v>
       </c>
       <c r="D320">
         <v>0</v>
       </c>
       <c r="E320">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="321" spans="1:5">
@@ -5230,13 +5230,13 @@
         <v>19</v>
       </c>
       <c r="C321">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D321">
         <v>0</v>
       </c>
       <c r="E321">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="322" spans="1:5">
@@ -5245,13 +5245,13 @@
         <v>20</v>
       </c>
       <c r="C322">
-        <v>104365.375</v>
+        <v>141639.4</v>
       </c>
       <c r="D322">
         <v>0</v>
       </c>
       <c r="E322">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="323" spans="1:5">
@@ -5260,13 +5260,13 @@
         <v>21</v>
       </c>
       <c r="C323">
-        <v>94265.5</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D323">
         <v>0</v>
       </c>
       <c r="E323">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="324" spans="1:5">
@@ -5275,13 +5275,13 @@
         <v>22</v>
       </c>
       <c r="C324">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D324">
         <v>0</v>
       </c>
       <c r="E324">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="325" spans="1:5">
@@ -5290,13 +5290,13 @@
         <v>23</v>
       </c>
       <c r="C325">
-        <v>100998.75</v>
+        <v>141639.4</v>
       </c>
       <c r="D325">
         <v>0</v>
       </c>
       <c r="E325">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="326" spans="1:5">
@@ -5305,13 +5305,13 @@
         <v>24</v>
       </c>
       <c r="C326">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D326">
         <v>0</v>
       </c>
       <c r="E326">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="327" spans="1:5">
@@ -5320,13 +5320,13 @@
         <v>25</v>
       </c>
       <c r="C327">
-        <v>100998.75</v>
+        <v>141639.4</v>
       </c>
       <c r="D327">
         <v>0</v>
       </c>
       <c r="E327">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="328" spans="1:5">
@@ -5335,13 +5335,13 @@
         <v>26</v>
       </c>
       <c r="C328">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D328">
         <v>0</v>
       </c>
       <c r="E328">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="329" spans="1:5">
@@ -5350,13 +5350,13 @@
         <v>27</v>
       </c>
       <c r="C329">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D329">
         <v>0</v>
       </c>
       <c r="E329">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="330" spans="1:5">
@@ -5365,13 +5365,13 @@
         <v>28</v>
       </c>
       <c r="C330">
-        <v>100998.75</v>
+        <v>132196.7733333333</v>
       </c>
       <c r="D330">
         <v>0</v>
       </c>
       <c r="E330">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="331" spans="1:5">
@@ -5380,13 +5380,13 @@
         <v>29</v>
       </c>
       <c r="C331">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D331">
         <v>0</v>
       </c>
       <c r="E331">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="332" spans="1:5">
@@ -5395,13 +5395,13 @@
         <v>30</v>
       </c>
       <c r="C332">
-        <v>100998.75</v>
+        <v>141639.4</v>
       </c>
       <c r="D332">
         <v>0</v>
       </c>
       <c r="E332">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="333" spans="1:5">
@@ -5410,13 +5410,13 @@
         <v>31</v>
       </c>
       <c r="C333">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D333">
         <v>0</v>
       </c>
       <c r="E333">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="334" spans="1:5">
@@ -5425,13 +5425,13 @@
         <v>32</v>
       </c>
       <c r="C334">
-        <v>104365.375</v>
+        <v>141639.4</v>
       </c>
       <c r="D334">
         <v>0</v>
       </c>
       <c r="E334">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="335" spans="1:5">
@@ -5440,13 +5440,13 @@
         <v>33</v>
       </c>
       <c r="C335">
-        <v>94265.5</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D335">
         <v>0</v>
       </c>
       <c r="E335">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="336" spans="1:5">
@@ -5455,13 +5455,13 @@
         <v>34</v>
       </c>
       <c r="C336">
-        <v>104365.375</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D336">
         <v>0</v>
       </c>
       <c r="E336">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="337" spans="1:5">
@@ -5470,13 +5470,13 @@
         <v>35</v>
       </c>
       <c r="C337">
-        <v>100998.75</v>
+        <v>141639.4</v>
       </c>
       <c r="D337">
-        <v>10539000</v>
+        <v>0</v>
       </c>
       <c r="E337">
-        <v>10539000</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="338" spans="1:5">
@@ -5485,13 +5485,13 @@
         <v>36</v>
       </c>
       <c r="C338">
-        <v>0</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D338">
         <v>0</v>
       </c>
       <c r="E338">
-        <v>0</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="339" spans="1:5">
@@ -5500,13 +5500,13 @@
         <v>37</v>
       </c>
       <c r="C339">
-        <v>0</v>
+        <v>141639.4</v>
       </c>
       <c r="D339">
         <v>0</v>
       </c>
       <c r="E339">
-        <v>0</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="340" spans="1:5">
@@ -5515,13 +5515,13 @@
         <v>38</v>
       </c>
       <c r="C340">
-        <v>0</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D340">
         <v>0</v>
       </c>
       <c r="E340">
-        <v>0</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="341" spans="1:5">
@@ -5530,13 +5530,13 @@
         <v>39</v>
       </c>
       <c r="C341">
-        <v>0</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D341">
         <v>0</v>
       </c>
       <c r="E341">
-        <v>0</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="342" spans="1:5">
@@ -5545,13 +5545,13 @@
         <v>40</v>
       </c>
       <c r="C342">
-        <v>0</v>
+        <v>132196.7733333333</v>
       </c>
       <c r="D342">
         <v>0</v>
       </c>
       <c r="E342">
-        <v>0</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="343" spans="1:5">
@@ -5560,13 +5560,13 @@
         <v>41</v>
       </c>
       <c r="C343">
-        <v>0</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D343">
         <v>0</v>
       </c>
       <c r="E343">
-        <v>0</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="344" spans="1:5">
@@ -5575,13 +5575,13 @@
         <v>42</v>
       </c>
       <c r="C344">
-        <v>0</v>
+        <v>141639.4</v>
       </c>
       <c r="D344">
         <v>0</v>
       </c>
       <c r="E344">
-        <v>0</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="345" spans="1:5">
@@ -5590,13 +5590,13 @@
         <v>43</v>
       </c>
       <c r="C345">
-        <v>0</v>
+        <v>146360.7133333333</v>
       </c>
       <c r="D345">
-        <v>0</v>
+        <v>16296000</v>
       </c>
       <c r="E345">
-        <v>0</v>
+        <v>16296000</v>
       </c>
     </row>
     <row r="346" spans="1:5">

</xml_diff>